<commit_message>
Added a first draft for the BalloonBox subsystem and its commands.
</commit_message>
<xml_diff>
--- a/BranchementsRobot2019.xlsx
+++ b/BranchementsRobot2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fenix\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fenix\workspace\robot2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACE9525-47F8-4730-906E-2E30310BED4B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E11DFEE-4AA1-4297-B764-309FFF0D1788}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1C6C62-AAC3-4D46-9165-7FB5851C2C68}"/>
+    <workbookView xWindow="4884" yWindow="1620" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1C6C62-AAC3-4D46-9165-7FB5851C2C68}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t xml:space="preserve">Robot </t>
   </si>
@@ -102,7 +102,28 @@
     <t>Power distribution Panel</t>
   </si>
   <si>
-    <t>pas assigné</t>
+    <t>Pigeon IMU</t>
+  </si>
+  <si>
+    <t>Pigeon</t>
+  </si>
+  <si>
+    <t>Pigeon centrale inertielle</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Box position</t>
+  </si>
+  <si>
+    <t>2 limit switch</t>
+  </si>
+  <si>
+    <t>Intake roller</t>
+  </si>
+  <si>
+    <t>Sensor</t>
   </si>
 </sst>
 </file>
@@ -454,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDC305A-8A81-4471-9FDB-C00527822415}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,6 +508,9 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -524,6 +548,9 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -647,10 +674,13 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -664,10 +694,27 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated wiring of talons
</commit_message>
<xml_diff>
--- a/BranchementsRobot2019.xlsx
+++ b/BranchementsRobot2019.xlsx
@@ -8,30 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fenix\workspace\robot2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E11DFEE-4AA1-4297-B764-309FFF0D1788}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FE396F-AA2C-4636-8BFD-A6E8E54D0033}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4884" yWindow="1620" windowWidth="17280" windowHeight="8964" xr2:uid="{BF1C6C62-AAC3-4D46-9165-7FB5851C2C68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BF1C6C62-AAC3-4D46-9165-7FB5851C2C68}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t xml:space="preserve">Robot </t>
   </si>
@@ -114,16 +108,19 @@
     <t>Box</t>
   </si>
   <si>
-    <t>Box position</t>
-  </si>
-  <si>
-    <t>2 limit switch</t>
-  </si>
-  <si>
     <t>Intake roller</t>
   </si>
   <si>
     <t>Sensor</t>
+  </si>
+  <si>
+    <t>Climber active wheel</t>
+  </si>
+  <si>
+    <t>Limit switches</t>
+  </si>
+  <si>
+    <t>Intake Position</t>
   </si>
 </sst>
 </file>
@@ -475,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDC305A-8A81-4471-9FDB-C00527822415}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -626,7 +623,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -674,13 +671,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,7 +691,7 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -715,6 +709,26 @@
       </c>
       <c r="E15" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>